<commit_message>
Creacion de filtros x profesor y modificacion de paginas
</commit_message>
<xml_diff>
--- a/TPI/uploads/ExcelLocal.xlsx
+++ b/TPI/uploads/ExcelLocal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jere\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02CEB66-D065-4BF2-92DE-DDE53B0D9EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E542BB-5BF8-4EF0-9031-7EF7AC155A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2655" windowWidth="15375" windowHeight="7860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Legajo</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>AC</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>Jueves</t>
+  </si>
+  <si>
+    <t>Viernes</t>
   </si>
 </sst>
 </file>
@@ -384,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,6 +481,57 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E5" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E7" s="1">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se validaron las consultas de las materias a las que el docente esta dando clases
</commit_message>
<xml_diff>
--- a/TPI/uploads/ExcelLocal.xlsx
+++ b/TPI/uploads/ExcelLocal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jere\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E542BB-5BF8-4EF0-9031-7EF7AC155A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D3B20E-E5BE-4B41-B278-DBE0EF7D856A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Legajo</t>
   </si>
@@ -54,18 +54,6 @@
     <t>AM1</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>SO</t>
-  </si>
-  <si>
     <t>AED</t>
   </si>
   <si>
@@ -73,6 +61,24 @@
   </si>
   <si>
     <t>Viernes</t>
+  </si>
+  <si>
+    <t>ACO</t>
+  </si>
+  <si>
+    <t>FI1</t>
+  </si>
+  <si>
+    <t>SYO</t>
+  </si>
+  <si>
+    <t>MAD</t>
+  </si>
+  <si>
+    <t>ADS</t>
+  </si>
+  <si>
+    <t>IYS</t>
   </si>
 </sst>
 </file>
@@ -399,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +455,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -466,7 +472,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -483,13 +489,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3">
         <v>0.45833333333333331</v>
@@ -500,13 +506,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2">
         <v>0.83333333333333337</v>
@@ -517,7 +523,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -529,6 +535,40 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="E7" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E8" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E9" s="1">
         <v>25</v>
       </c>
     </row>

</xml_diff>